<commit_message>
Changed excel sheet format, added finish attachments option
</commit_message>
<xml_diff>
--- a/RFQ_template_fin.xlsx
+++ b/RFQ_template_fin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saggarwal\PythonProjects\email_app_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D388DF6-3D07-4830-B77E-67A39B9F72EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C38E9A5-5E16-45D7-AFB0-FF7AF5CD6932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28110" yWindow="855" windowWidth="25860" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26790" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Part Number</t>
   </si>
@@ -82,13 +82,25 @@
   </si>
   <si>
     <t>US Dollar</t>
+  </si>
+  <si>
+    <t>Company Name:</t>
+  </si>
+  <si>
+    <t>Your Name:</t>
+  </si>
+  <si>
+    <t>Email ID:</t>
+  </si>
+  <si>
+    <t>Phone Number:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +116,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,13 +157,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -167,8 +203,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:O2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A5:O6" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A5:O6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part Number"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Description"/>
@@ -507,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,97 +568,121 @@
     <col min="15" max="15" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D6">
         <v>6.3E-2</v>
       </c>
-      <c r="E2">
+      <c r="E6">
         <v>1.25</v>
       </c>
-      <c r="F2">
+      <c r="F6">
         <v>3.5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2">
+      <c r="H6">
         <v>100</v>
       </c>
-      <c r="I2">
+      <c r="I6">
         <v>25</v>
       </c>
-      <c r="J2">
+      <c r="J6">
         <v>10</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K6" s="3">
         <v>45534</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L6" t="s">
         <v>19</v>
       </c>
-      <c r="M2">
+      <c r="M6">
         <v>50</v>
       </c>
-      <c r="N2">
+      <c r="N6">
         <v>5</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O6" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>